<commit_message>
Created code to run on PRIME cluster and implemented parallel processing
</commit_message>
<xml_diff>
--- a/Timeline.xlsx
+++ b/Timeline.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aarhusuniversitet-my.sharepoint.com/personal/au518895_uni_au_dk/Documents/Speciale/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim\OneDrive - Aarhus universitet\Speciale\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="8_{FEB2071E-969A-4FBB-B8AA-CBE65637D075}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{4E318F79-C104-4197-B59E-D5CAFAFC4C5F}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="8_{FEB2071E-969A-4FBB-B8AA-CBE65637D075}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{E4DF912E-F01B-4D15-B6A3-9BB84FBFBA99}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4532B92F-75B5-48F8-AA98-EC43B78D7B99}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{4532B92F-75B5-48F8-AA98-EC43B78D7B99}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="21">
   <si>
     <t>Final Draft</t>
   </si>
@@ -109,7 +109,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -137,6 +137,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -215,7 +221,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -238,6 +244,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -554,8 +561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4506EE92-4598-4F30-9295-0D096DC6786B}">
   <dimension ref="A2:U39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,6 +579,15 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -872,7 +888,7 @@
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
+      <c r="G11" s="14"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="4" t="s">
@@ -900,8 +916,8 @@
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
       <c r="J12" s="4" t="s">
         <v>7</v>
       </c>
@@ -1423,6 +1439,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100E400970CD30FDE419634157DC0979CEB" ma:contentTypeVersion="6" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="9591bd262819d37b8270f0eb02779584">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c60c6253-16de-4fa8-ae79-8e38ec3056bb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d8994168d28efc439daf02f258898dfa" ns3:_="">
     <xsd:import namespace="c60c6253-16de-4fa8-ae79-8e38ec3056bb"/>
@@ -1580,22 +1611,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12907AFD-6107-40D7-B8BE-3E52530776D6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="c60c6253-16de-4fa8-ae79-8e38ec3056bb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31DD9905-CC87-4BD2-9431-13D0F302382C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98234A04-3E10-4586-86F4-D732B65C6EBF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1611,28 +1651,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31DD9905-CC87-4BD2-9431-13D0F302382C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12907AFD-6107-40D7-B8BE-3E52530776D6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="c60c6253-16de-4fa8-ae79-8e38ec3056bb"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Data from 4D study included and post processing updated
</commit_message>
<xml_diff>
--- a/Timeline.xlsx
+++ b/Timeline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim\OneDrive - Aarhus universitet\Speciale\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="8_{FEB2071E-969A-4FBB-B8AA-CBE65637D075}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{E4DF912E-F01B-4D15-B6A3-9BB84FBFBA99}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="8_{FEB2071E-969A-4FBB-B8AA-CBE65637D075}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{9561D15D-BABC-4F75-A385-802EB1265701}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{4532B92F-75B5-48F8-AA98-EC43B78D7B99}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4532B92F-75B5-48F8-AA98-EC43B78D7B99}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="21">
   <si>
     <t>Final Draft</t>
   </si>
@@ -561,8 +561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4506EE92-4598-4F30-9295-0D096DC6786B}">
   <dimension ref="A2:U39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,6 +588,21 @@
         <v>14</v>
       </c>
       <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1439,21 +1454,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100E400970CD30FDE419634157DC0979CEB" ma:contentTypeVersion="6" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="9591bd262819d37b8270f0eb02779584">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c60c6253-16de-4fa8-ae79-8e38ec3056bb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d8994168d28efc439daf02f258898dfa" ns3:_="">
     <xsd:import namespace="c60c6253-16de-4fa8-ae79-8e38ec3056bb"/>
@@ -1611,31 +1611,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12907AFD-6107-40D7-B8BE-3E52530776D6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="c60c6253-16de-4fa8-ae79-8e38ec3056bb"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31DD9905-CC87-4BD2-9431-13D0F302382C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98234A04-3E10-4586-86F4-D732B65C6EBF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1651,4 +1642,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31DD9905-CC87-4BD2-9431-13D0F302382C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12907AFD-6107-40D7-B8BE-3E52530776D6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="c60c6253-16de-4fa8-ae79-8e38ec3056bb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>